<commit_message>
feat: Implement multi-record support in layout normalization and validation
- Added functionality to handle multi-record layouts in `layout_normalizer.py`, allowing for position resets based on record types.
- Enhanced validation in `layout_parser.py` to check for overlaps within the same record type for multi-record files.
- Updated `multi_record_validator.py` to reset positions for each record type and added a method to parse preview lines from files.
- Introduced new test file `test_multirecord.xlsx` to validate multi-record functionality.
- Created multiple validation reports for the new layout structure, including statistics and error types.
- Removed outdated validation reports that are no longer relevant.
</commit_message>
<xml_diff>
--- a/layout_tipo_00.xlsx
+++ b/layout_tipo_00.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -508,7 +508,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -532,7 +532,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -556,7 +556,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -580,7 +580,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>S</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>

</xml_diff>